<commit_message>
update code for convention
</commit_message>
<xml_diff>
--- a/output/DANH_MUC_DICH_VU.xlsx
+++ b/output/DANH_MUC_DICH_VU.xlsx
@@ -1170,7 +1170,7 @@
         </is>
       </c>
       <c r="T4" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="U4" t="inlineStr">
         <is>
@@ -1200,7 +1200,7 @@
       </c>
       <c r="AA4" t="inlineStr">
         <is>
-          <t>[{'id': 'ab660ea7-d879-480b-adf9-d50b1cf680d4'}, {'id': '4fd2a841-5293-484d-b5ba-ec0236294574'}, {'id': 'd27216c4-ba32-4973-b2ce-9b04af6ff585'}, {'id': '47ff8592-f0f8-4311-a1ed-663587ed2f33'}]</t>
+          <t>[{'id': 'ab660ea7-d879-480b-adf9-d50b1cf680d4'}, {'id': '4fd2a841-5293-484d-b5ba-ec0236294574'}, {'id': 'd27216c4-ba32-4973-b2ce-9b04af6ff585'}, {'id': '47ff8592-f0f8-4311-a1ed-663587ed2f33'}, {'id': '4d1ce8ad-da1c-43bc-a0a1-96aa4c0cce3d'}]</t>
         </is>
       </c>
       <c r="AB4" t="b">
@@ -6912,7 +6912,7 @@
         </is>
       </c>
       <c r="T31" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="U31" t="inlineStr">
         <is>
@@ -6944,7 +6944,7 @@
       </c>
       <c r="AA31" t="inlineStr">
         <is>
-          <t>[{'id': 'd0ea2871-65bd-47bf-9203-7de1d77ed91e'}, {'id': 'b704a0ef-5a90-4ec1-92fa-3b889937347b'}]</t>
+          <t>[{'id': 'd0ea2871-65bd-47bf-9203-7de1d77ed91e'}, {'id': 'b704a0ef-5a90-4ec1-92fa-3b889937347b'}, {'id': '6d613630-ae9d-4877-8c65-fce6533a0854'}]</t>
         </is>
       </c>
       <c r="AB31" t="b">
@@ -8220,7 +8220,7 @@
         </is>
       </c>
       <c r="T37" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="U37" t="inlineStr">
         <is>
@@ -8252,7 +8252,7 @@
       </c>
       <c r="AA37" t="inlineStr">
         <is>
-          <t>[{'id': '9710180c-11ab-4697-bd65-bc5bc6be0fa6'}, {'id': '946c11fc-ceaf-47d8-bf04-f50a03e741bb'}, {'id': '0cc71c84-16a1-41dd-98f4-bb6829014155'}, {'id': '999f7a1a-951e-4ec9-b9bf-0ee7b79b32b4'}]</t>
+          <t>[{'id': '9710180c-11ab-4697-bd65-bc5bc6be0fa6'}, {'id': '946c11fc-ceaf-47d8-bf04-f50a03e741bb'}, {'id': '0cc71c84-16a1-41dd-98f4-bb6829014155'}, {'id': '999f7a1a-951e-4ec9-b9bf-0ee7b79b32b4'}, {'id': '6f2705c2-4b83-4320-b7dc-ab284a15c675'}]</t>
         </is>
       </c>
       <c r="AB37" t="b">

</xml_diff>